<commit_message>
fixing unit testing semi automation
</commit_message>
<xml_diff>
--- a/src/test/resources/data-test/akses.xlsx
+++ b/src/test/resources/data-test/akses.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\SPRINGBOOT-PT-DIKA\pcmspringbootrestapidika\src\test\resources\data-test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37AC73CE-3752-4075-B92B-64D12CE2DA88}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFBCB8AA-1D43-47FA-89D0-D71C1C24837C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{47EA533E-3F0C-4ED1-A111-B65235F9FF84}"/>
   </bookViews>
@@ -25,22 +25,22 @@
     <t>nama</t>
   </si>
   <si>
-    <t>Akses7</t>
+    <t>Akses1</t>
   </si>
   <si>
-    <t>Akses8</t>
+    <t>Akses2</t>
   </si>
   <si>
-    <t>Akses9</t>
+    <t>Akses3</t>
   </si>
   <si>
-    <t>Akses10</t>
+    <t>Akses4</t>
   </si>
   <si>
-    <t>Akses11</t>
+    <t>Akses5</t>
   </si>
   <si>
-    <t>Akses12</t>
+    <t>Akses6</t>
   </si>
 </sst>
 </file>
@@ -890,7 +890,7 @@
   <dimension ref="A1:A7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A7"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>